<commit_message>
figure (plus corresponding markdown and data files) changes per reviewer suggestions - Figures 1, S1A edited, added S1B
</commit_message>
<xml_diff>
--- a/Figures/Table_1_raw_cvv.xlsx
+++ b/Figures/Table_1_raw_cvv.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/divyav/Dropbox/work/Projects/P2_Swine/2019_swine_NAm/analysis/7_WHO-VCM-CVV/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/divyav/Dropbox/Work-upto2021/RVC-postdoc-related/Projects/P2_Swine/2019_swine_NAm/MS_swineNAm_DV/1_revision/h1-risk-pipeline/Figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89102C33-B358-114A-B15D-0BF050BB0D37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C05356-F56E-494C-8CC8-3E2D3F3F79C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15900" xr2:uid="{13773821-9359-094E-8092-38E0E269EA87}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -364,25 +365,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -420,8 +419,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -448,10 +447,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -460,13 +459,13 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -484,26 +483,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,10 +816,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0307991E-A686-F44E-8526-B63EBF37ED1B}">
-  <dimension ref="A2:L22"/>
+  <dimension ref="B2:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -831,93 +829,85 @@
     <col min="3" max="3" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="7.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="1"/>
-    <col min="10" max="16384" width="10.83203125" style="56"/>
+    <col min="9" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="174" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="55" t="s">
+    <row r="2" spans="2:8" ht="174" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="53" t="s">
         <v>32</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="40" t="s">
+      <c r="F2" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="39" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="42" t="s">
+    <row r="3" spans="2:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="21" t="s">
+      <c r="D3" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="8">
         <v>5120</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="9">
         <v>2560</v>
       </c>
-      <c r="G3" s="50" t="s">
+      <c r="G3" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="46">
+      <c r="H3" s="44">
         <v>1280</v>
       </c>
-      <c r="L3" s="56">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="43" t="s">
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="41" t="s">
         <v>16</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="12">
         <v>160</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="13">
         <v>160</v>
       </c>
       <c r="G4" s="4">
         <v>10</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="11">
         <v>80</v>
       </c>
-      <c r="L4" s="56">
-        <f>L3*2</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="43" t="s">
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="43" t="s">
+      <c r="C5" s="41" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="10">
         <v>40</v>
       </c>
       <c r="F5" s="4">
@@ -926,25 +916,21 @@
       <c r="G5" s="4">
         <v>320</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="11">
         <v>2560</v>
       </c>
-      <c r="L5" s="56">
-        <f t="shared" ref="L5:L12" si="0">L4*2</f>
-        <v>160</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="43" t="s">
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="41" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="10">
         <v>20</v>
       </c>
       <c r="F6" s="4">
@@ -953,133 +939,113 @@
       <c r="G6" s="4">
         <v>80</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="11">
         <v>1280</v>
       </c>
-      <c r="L6" s="56">
-        <f t="shared" si="0"/>
-        <v>320</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="43" t="s">
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="41" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="10" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="16">
+      <c r="G7" s="14">
         <v>1280</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="11">
         <v>10</v>
       </c>
-      <c r="L7" s="56">
-        <f t="shared" si="0"/>
-        <v>640</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="43" t="s">
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="41" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="10" t="s">
         <v>3</v>
       </c>
       <c r="F8" s="4">
         <v>10</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="15">
         <v>1280</v>
       </c>
-      <c r="H8" s="13">
-        <v>20</v>
-      </c>
-      <c r="L8" s="56">
-        <f t="shared" si="0"/>
-        <v>1280</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="43" t="s">
+      <c r="H8" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="41" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="10">
         <v>10</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="15">
         <v>160</v>
       </c>
-      <c r="H9" s="13">
-        <v>20</v>
-      </c>
-      <c r="L9" s="56">
-        <f t="shared" si="0"/>
-        <v>2560</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="43" t="s">
+      <c r="H9" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="41" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="10">
         <v>10</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="18">
+      <c r="G10" s="16">
         <v>320</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="11">
         <v>10</v>
       </c>
-      <c r="L10" s="56">
-        <f t="shared" si="0"/>
-        <v>5120</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="43" t="s">
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="41" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="10">
         <v>80</v>
       </c>
       <c r="F11" s="4">
@@ -1088,204 +1054,172 @@
       <c r="G11" s="4">
         <v>160</v>
       </c>
-      <c r="H11" s="16">
+      <c r="H11" s="14">
         <v>10240</v>
       </c>
-      <c r="L11" s="56">
-        <f t="shared" si="0"/>
-        <v>10240</v>
-      </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="44" t="s">
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="27" t="s">
+      <c r="C12" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="14">
+      <c r="E12" s="12">
         <v>80</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="26">
         <v>40</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="26">
         <v>160</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="16">
         <v>5120</v>
       </c>
-      <c r="L12" s="56">
-        <f t="shared" si="0"/>
-        <v>20480</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" s="1" customFormat="1" ht="116" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="55" t="s">
+    </row>
+    <row r="15" spans="2:8" ht="116" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="41" t="s">
+      <c r="G15" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="56"/>
-    </row>
-    <row r="16" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="42" t="s">
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="14">
         <v>640</v>
       </c>
-      <c r="F16" s="50">
-        <v>20</v>
-      </c>
-      <c r="G16" s="46">
-        <v>20</v>
-      </c>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-    </row>
-    <row r="17" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="43" t="s">
+      <c r="F16" s="48">
+        <v>20</v>
+      </c>
+      <c r="G16" s="44">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C17" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="43" t="s">
+      <c r="C17" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="16">
         <v>80</v>
       </c>
       <c r="F17" s="4">
         <v>20</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="11">
         <v>80</v>
       </c>
-      <c r="J17" s="56"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="56"/>
-    </row>
-    <row r="18" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="43" t="s">
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="43" t="s">
+      <c r="C18" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="10">
         <v>40</v>
       </c>
       <c r="F18" s="4">
         <v>20</v>
       </c>
-      <c r="G18" s="13">
-        <v>20</v>
-      </c>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-    </row>
-    <row r="19" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="43" t="s">
+      <c r="G18" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="43" t="s">
+      <c r="C19" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="43" t="s">
+      <c r="D19" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="12">
+      <c r="E19" s="10">
         <v>80</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="8">
         <v>640</v>
       </c>
-      <c r="G19" s="46">
+      <c r="G19" s="44">
         <v>160</v>
       </c>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
-    </row>
-    <row r="20" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="43" t="s">
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="43" t="s">
+      <c r="C20" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="10">
         <v>40</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="10">
         <v>160</v>
       </c>
-      <c r="G20" s="38">
+      <c r="G20" s="36">
         <v>1280</v>
       </c>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-    </row>
-    <row r="21" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="44" t="s">
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="44" t="s">
+      <c r="C21" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="14">
-        <v>20</v>
-      </c>
-      <c r="F21" s="14">
+      <c r="E21" s="12">
+        <v>20</v>
+      </c>
+      <c r="F21" s="12">
         <v>320</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G21" s="13">
         <v>1280</v>
       </c>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="56"/>
-    </row>
-    <row r="22" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="9"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="9"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
       <c r="G22" s="4"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1295,7 +1229,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DA8E929-CAF9-5D45-98DB-9CC6A5F473D0}">
-  <dimension ref="A2:L26"/>
+  <dimension ref="B2:L26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:H3"/>
@@ -1303,298 +1237,295 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="6"/>
-    <col min="2" max="2" width="34.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="7.83203125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="6"/>
-    <col min="10" max="16384" width="10.83203125" style="7"/>
+    <col min="2" max="2" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="7.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="21" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="E2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="20" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="32"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="27" t="s">
+      <c r="B3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="32" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="163" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="23"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="3"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="40" t="s">
+      <c r="F4" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="41" t="s">
+      <c r="H4" s="39" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="42" t="s">
+      <c r="B5" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="37">
+      <c r="E5" s="35">
         <v>5120</v>
       </c>
-      <c r="F5" s="38">
+      <c r="F5" s="36">
         <v>2560</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="11">
         <v>1280</v>
       </c>
-      <c r="L5" s="7">
+      <c r="L5">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="43" t="s">
+      <c r="B6" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="43" t="s">
+      <c r="C6" s="41" t="s">
         <v>16</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="10">
         <v>160</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="11">
         <v>160</v>
       </c>
       <c r="G6" s="4">
         <v>10</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="11">
         <v>80</v>
       </c>
-      <c r="L6" s="7">
+      <c r="L6">
         <f>L5*2</f>
         <v>80</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="43" t="s">
+      <c r="C7" s="41" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="10">
         <v>40</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F7" s="11">
         <v>20</v>
       </c>
       <c r="G7" s="4">
         <v>320</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="11">
         <v>2560</v>
       </c>
-      <c r="L7" s="7">
+      <c r="L7">
         <f t="shared" ref="L7:L14" si="0">L6*2</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="41" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="14">
-        <v>20</v>
-      </c>
-      <c r="F8" s="15">
+      <c r="E8" s="12">
+        <v>20</v>
+      </c>
+      <c r="F8" s="13">
         <v>20</v>
       </c>
       <c r="G8" s="4">
         <v>80</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="11">
         <v>1280</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8">
         <f t="shared" si="0"/>
         <v>320</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="41" t="s">
         <v>15</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="10" t="s">
         <v>3</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G9" s="14">
         <v>1280</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="11">
         <v>10</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9">
         <f t="shared" si="0"/>
         <v>640</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="43" t="s">
+      <c r="C10" s="41" t="s">
         <v>16</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="10" t="s">
         <v>3</v>
       </c>
       <c r="F10" s="4">
         <v>10</v>
       </c>
-      <c r="G10" s="17">
+      <c r="G10" s="15">
         <v>1280</v>
       </c>
-      <c r="H10" s="13">
-        <v>20</v>
-      </c>
-      <c r="L10" s="7">
+      <c r="H10" s="11">
+        <v>20</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="0"/>
         <v>1280</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="41" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="10">
         <v>10</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G11" s="17">
+      <c r="G11" s="15">
         <v>160</v>
       </c>
-      <c r="H11" s="13">
-        <v>20</v>
-      </c>
-      <c r="L11" s="7">
+      <c r="H11" s="11">
+        <v>20</v>
+      </c>
+      <c r="L11">
         <f t="shared" si="0"/>
         <v>2560</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="43" t="s">
+      <c r="C12" s="41" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="12">
+      <c r="E12" s="10">
         <v>10</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="18">
+      <c r="G12" s="16">
         <v>320</v>
       </c>
-      <c r="H12" s="13">
+      <c r="H12" s="11">
         <v>10</v>
       </c>
-      <c r="L12" s="7">
+      <c r="L12">
         <f t="shared" si="0"/>
         <v>5120</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="41" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="10">
         <v>80</v>
       </c>
       <c r="F13" s="4">
@@ -1603,211 +1534,211 @@
       <c r="G13" s="4">
         <v>160</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="14">
         <v>10240</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13">
         <f t="shared" si="0"/>
         <v>10240</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="27" t="s">
+      <c r="C14" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E14" s="14">
+      <c r="E14" s="12">
         <v>80</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="26">
         <v>40</v>
       </c>
-      <c r="G14" s="28">
+      <c r="G14" s="26">
         <v>160</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="16">
         <v>5120</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L14">
         <f t="shared" si="0"/>
         <v>20480</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="21" t="s">
+      <c r="C17" s="45"/>
+      <c r="D17" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E17" s="29" t="s">
+      <c r="E17" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="48" t="s">
+      <c r="G17" s="46" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="51"/>
-      <c r="C18" s="52"/>
-      <c r="D18" s="27" t="s">
+      <c r="B18" s="49"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="53" t="s">
+      <c r="E18" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="F18" s="27" t="s">
+      <c r="F18" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G18" s="31" t="s">
+      <c r="G18" s="29" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="105" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="49"/>
-      <c r="E19" s="54" t="s">
+      <c r="B19" s="47"/>
+      <c r="E19" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G19" s="24" t="s">
+      <c r="G19" s="22" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="42" t="s">
+      <c r="B20" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="14">
         <v>640</v>
       </c>
-      <c r="F20" s="50">
-        <v>20</v>
-      </c>
-      <c r="G20" s="46">
+      <c r="F20" s="48">
+        <v>20</v>
+      </c>
+      <c r="G20" s="44">
         <v>20</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="25" t="s">
+      <c r="C21" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="16">
         <v>80</v>
       </c>
       <c r="F21" s="4">
         <v>20</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="11">
         <v>80</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="25" t="s">
+      <c r="C22" s="41" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E22" s="12">
+      <c r="E22" s="10">
         <v>40</v>
       </c>
       <c r="F22" s="4">
         <v>20</v>
       </c>
-      <c r="G22" s="13">
+      <c r="G22" s="11">
         <v>20</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="43" t="s">
+      <c r="C23" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E23" s="12">
+      <c r="E23" s="10">
         <v>80</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23" s="8">
         <v>640</v>
       </c>
-      <c r="G23" s="46">
+      <c r="G23" s="44">
         <v>160</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="43" t="s">
+      <c r="C24" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="12">
+      <c r="E24" s="10">
         <v>40</v>
       </c>
-      <c r="F24" s="12">
+      <c r="F24" s="10">
         <v>160</v>
       </c>
-      <c r="G24" s="38">
+      <c r="G24" s="36">
         <v>1280</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="26" t="s">
+      <c r="C25" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="14">
-        <v>20</v>
-      </c>
-      <c r="F25" s="14">
+      <c r="E25" s="12">
+        <v>20</v>
+      </c>
+      <c r="F25" s="12">
         <v>320</v>
       </c>
-      <c r="G25" s="15">
+      <c r="G25" s="13">
         <v>1280</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
       <c r="G26" s="4"/>
     </row>
   </sheetData>

</xml_diff>